<commit_message>
made ms workplan for July/Aug
</commit_message>
<xml_diff>
--- a/ms/PlatyMS_workplan.xlsx
+++ b/ms/PlatyMS_workplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17300" tabRatio="500"/>
+    <workbookView xWindow="-100" yWindow="0" windowWidth="28820" windowHeight="14080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t xml:space="preserve">Platy Manuscript to do: </t>
   </si>
@@ -45,12 +45,6 @@
     <t>Done!! :-)</t>
   </si>
   <si>
-    <t>Make one first week (i.e. done by Fri. Aug. 21)</t>
-  </si>
-  <si>
-    <t>Make one second week (i.e. done by Fri. Aug. 28)</t>
-  </si>
-  <si>
     <t>Polished version of Figure 2 and caption (i.e. exact formats needed for Nature)</t>
   </si>
   <si>
@@ -64,13 +58,55 @@
   </si>
   <si>
     <t>Extended Data Figure 1 and caption (i.e. multi-panel photos of ~3 other individul corals (e.g. 3 other species, or 2 other species + a 2nd Platy)</t>
+  </si>
+  <si>
+    <t>Re-run bioinformatics pipeline as double check</t>
+  </si>
+  <si>
+    <t>Plug away at over the new week (i.e. have done by Friday July 21).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make week of July 24-28th  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Needs to be completed before can make Figures 2 or 3. </t>
+  </si>
+  <si>
+    <t>Extended Data Figure 2 - rank abundance plot (?) showing dominance/evenness of Clade C vs. D (4 panels - low/high disturbance, before/after El Niño)</t>
+  </si>
+  <si>
+    <t>Writing</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Figures</t>
+  </si>
+  <si>
+    <t>Goal: Have rough version of main text; have all figures (incl. figure captions, extended data figures), tables, Methods complete by Aug. 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tables </t>
+  </si>
+  <si>
+    <t>have a think about if it would be useful to have any other extended data figures or tables in the supp. Mat.</t>
+  </si>
+  <si>
+    <t>Keep working on writing in main text (doing the paragraphs that describe each of the figures first)</t>
+  </si>
+  <si>
+    <t>Suggest to work on this for max. 1 hour per day, when freshest for writing :-)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">progress by Aug. 2 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,16 +146,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -127,8 +177,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -140,23 +216,53 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -486,85 +592,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
-    <col min="2" max="2" width="40.1640625" customWidth="1"/>
+    <col min="1" max="1" width="68.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
     <col min="3" max="3" width="80.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="16" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:3" ht="16" thickBot="1">
+      <c r="A2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="7"/>
+    </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30">
+      <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
-        <v>13</v>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish fig 2 and caption
</commit_message>
<xml_diff>
--- a/ms/PlatyMS_workplan.xlsx
+++ b/ms/PlatyMS_workplan.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Documents\Data_Analysis\KI_Platy\ms\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="0" windowWidth="28820" windowHeight="14080" tabRatio="500"/>
+    <workbookView xWindow="-102" yWindow="0" windowWidth="28818" windowHeight="14082" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -105,7 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -155,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +170,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,7 +244,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -241,6 +258,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -267,6 +292,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -594,33 +627,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="68.33203125" customWidth="1"/>
+    <col min="1" max="1" width="68.34765625" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="80.6640625" customWidth="1"/>
+    <col min="3" max="3" width="80.6484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1">
+    <row r="1" spans="1:3" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" thickBot="1">
+    <row r="2" spans="1:3" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -631,117 +664,121 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="3" t="s">
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="30">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A20" s="12" t="s">
         <v>23</v>
       </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated workplan before call w Ruth
</commit_message>
<xml_diff>
--- a/ms/PlatyMS_workplan.xlsx
+++ b/ms/PlatyMS_workplan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-102" yWindow="0" windowWidth="28818" windowHeight="14082" tabRatio="500"/>
+    <workbookView xWindow="-102" yWindow="0" windowWidth="13062" windowHeight="8808" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t xml:space="preserve">Platy Manuscript to do: </t>
   </si>
@@ -105,13 +105,112 @@
   </si>
   <si>
     <t xml:space="preserve">progress by Aug. 2 </t>
+  </si>
+  <si>
+    <t>Add error bars to figure 2</t>
+  </si>
+  <si>
+    <t>Caption for extended figure 2</t>
+  </si>
+  <si>
+    <t>Rarify for extended data figure 2</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Write cover letter</t>
+  </si>
+  <si>
+    <t>Julia and Danielle to review methods section</t>
+  </si>
+  <si>
+    <t>Finish up indicator species analysis (check on what else could/should be done with multipatt object)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decide whether unifrac needs to be jackknifed or not </t>
+  </si>
+  <si>
+    <t>Main text draft - send to Julia and Ruth</t>
+  </si>
+  <si>
+    <t>Complete by Wednesday, August 16</t>
+  </si>
+  <si>
+    <t>Julia review by Aug. 16, and then Danielle and Julia meet on Aug 16 to discuss (that way Danielle can incorporate changes by Friday Aug 18th)</t>
+  </si>
+  <si>
+    <t>Complete by Friday, August 18</t>
+  </si>
+  <si>
+    <t>Work on manuscript consistently (1 hour a day) to push as far forward as possible by Fri Aug 18</t>
+  </si>
+  <si>
+    <t>Complete on Aug 11th (as long as there are no problems)</t>
+  </si>
+  <si>
+    <t>Danielle to finish after Skype call with Ruth and Julia</t>
+  </si>
+  <si>
+    <t>Complete by Monday, August 14th</t>
+  </si>
+  <si>
+    <t>Work on starting Aug 11th if I have time, and finish up by Aug 14th at the latest (just need to do some reading about the R package to see if there are any easy additional steps I should add to strengthen this analysis</t>
+  </si>
+  <si>
+    <t>Complete by Tuesday, August 15th</t>
+  </si>
+  <si>
+    <t>Work on starting Aug 11th if I have time, and finish up by Aug 15th at the latest (need to read up a bit more on this to make sure that we don't need to jackknife the unifrac, and if we do, to ensure I do it correctly)</t>
+  </si>
+  <si>
+    <t>Revise all README files in the Git Repo</t>
+  </si>
+  <si>
+    <t>Completed!</t>
+  </si>
+  <si>
+    <t>Re-make extended data figure 2 with rareified results</t>
+  </si>
+  <si>
+    <t>Complete by Aug 11th (as long as there are no problems)</t>
+  </si>
+  <si>
+    <t>Danielle to finish after rarifying. If I run into any issues, I will finish this next week.</t>
+  </si>
+  <si>
+    <t>Complete by Friday, August 18th</t>
+  </si>
+  <si>
+    <t>Will probably do this before then, while taking a break from writing</t>
+  </si>
+  <si>
+    <t>Complete by Sept 13th, when Danielle returns from honeymoon</t>
+  </si>
+  <si>
+    <t>Julia/Ruth to write while Danielle is away</t>
+  </si>
+  <si>
+    <t>Finish formatting indicator species table for extended data</t>
+  </si>
+  <si>
+    <t>Revision of main text draft (Julia and Ruth)</t>
+  </si>
+  <si>
+    <t>Complete by Sept 14th, when Danielle returns from honeymoon</t>
+  </si>
+  <si>
+    <t>Julia and Ruth review the full manuscript between August 18th and Sept 14th</t>
+  </si>
+  <si>
+    <t>Goal: Have a complete rough draft done by Aug 18th, and reviewed by Julia/Ruth (+cover letter written) by September 14th.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,8 +258,17 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,12 +284,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -244,7 +346,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -259,10 +361,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -622,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -646,140 +753,286 @@
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A4" s="1" t="s">
+    <row r="3" spans="1:3" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>6</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>25</v>
+      <c r="A7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A9" s="4" t="s">
-        <v>19</v>
+      <c r="A9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A12" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A13" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="9"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A14" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A15" s="11" t="s">
-        <v>10</v>
+      <c r="A15" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>11</v>
+        <v>29</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A20" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A22" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A23" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A24" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A25" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A26" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A27" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A29" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A19" s="4" t="s">
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A31" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A20" s="11" t="s">
+    <row r="32" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A32" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A34" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="75" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="75" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
finish indicator taxa analysis, table, and caption
</commit_message>
<xml_diff>
--- a/ms/PlatyMS_workplan.xlsx
+++ b/ms/PlatyMS_workplan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t xml:space="preserve">Platy Manuscript to do: </t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>Re-make extended data figure 2 with rarefied results</t>
+  </si>
+  <si>
+    <t>Extended data table 1 caption</t>
   </si>
 </sst>
 </file>
@@ -747,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -887,13 +890,13 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -939,13 +942,13 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1017,47 +1020,58 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A31" s="3"/>
+    <row r="31" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A31" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A33" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A33" s="10" t="s">
+    <row r="34" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A34" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A35" s="12" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A36" s="12" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.6">
-      <c r="A36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="C37" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A39" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>